<commit_message>
* Created a more geographically aware ModelCanvas to replace the row/column dependent DemCanvas * Implemented ModelCanvas across 2D rendering, other render engines and shapefile rendering still incomplete
</commit_message>
<xml_diff>
--- a/jdem846/resources/Data Raster LatLong Calculations.xlsx
+++ b/jdem846/resources/Data Raster LatLong Calculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>1 a/s Set</t>
   </si>
@@ -64,13 +64,44 @@
   </si>
   <si>
     <t>Tile Size:</t>
+  </si>
+  <si>
+    <t>Raster:</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Raster LatLongBox</t>
+  </si>
+  <si>
+    <t>Buffer LatLongBox</t>
+  </si>
+  <si>
+    <t>Tile Lat Height</t>
+  </si>
+  <si>
+    <t>Tile Lon Width</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="175" formatCode="0.000000000000"/>
     <numFmt numFmtId="179" formatCode="0.0000000000000000"/>
     <numFmt numFmtId="180" formatCode="0.00000000000000000"/>
   </numFmts>
@@ -103,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -411,7 +443,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,10 +493,10 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>2.7777777779647002E-4</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>9.2592592593009003E-5</v>
       </c>
     </row>
@@ -472,22 +504,22 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <f>B6+(B3*B4)</f>
         <v>44.323888888653777</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <f>C6+(C3*C4)</f>
         <v>44.285833333303913</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>44.323888332117299</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <f>B5-D5</f>
         <v>5.5653647734743572E-7</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <f>C5-D5</f>
         <v>-3.8054998813386476E-2</v>
       </c>
@@ -496,20 +528,20 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>44.211666666424001</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>44.239629629600003</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>44.231388332300398</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <f>D6-B6</f>
         <v>1.9721665876396344E-2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <f>D6-C6</f>
         <v>-8.2412972996053213E-3</v>
       </c>
@@ -518,22 +550,22 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <f>B8 + (B2*B4)</f>
         <v>-71.244722218675577</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <f>C8 + (C2*C4)</f>
         <v>-71.279351851611708</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>-71.244812437835193</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <f>B7-D7</f>
         <v>9.0219159616822253E-5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <f>C7-D7</f>
         <v>-3.4539413776514039E-2</v>
       </c>
@@ -542,20 +574,20 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>-71.384722218684999</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>-71.325925925685993</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>-71.292219848815805</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <f>D8-B8</f>
         <v>9.2502369869194467E-2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <f>D8-C8</f>
         <v>3.3706076870188895E-2</v>
       </c>
@@ -569,7 +601,7 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <f>MIN(B4:C4)</f>
         <v>9.2592592593009003E-5</v>
       </c>
@@ -578,7 +610,7 @@
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <f>MAX(B5:C5)</f>
         <v>44.323888888653777</v>
       </c>
@@ -587,7 +619,7 @@
       <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <f>MIN(B6:C6)</f>
         <v>44.211666666424001</v>
       </c>
@@ -596,7 +628,7 @@
       <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <f>MAX(B7:C7)</f>
         <v>-71.244722218675577</v>
       </c>
@@ -605,7 +637,7 @@
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <f>MIN(B8:C8)</f>
         <v>-71.384722218684999</v>
       </c>
@@ -661,12 +693,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44.323888888653777</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44.285831541747001</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44.285831541747001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44.231388332300398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44.211666666424001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44.239627838134702</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44.239627838134702</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44.211758699770101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-71.244722218675577</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-71.279353660393099</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-71.279353660393099</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-71.292219848815805</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-71.384722218684999</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-71.325927734375</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-71.325927734375</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-71.384719848632798</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <f>B2-B3</f>
+        <v>0.11222222222977507</v>
+      </c>
+      <c r="C7" s="1">
+        <f>C2-C3</f>
+        <v>4.6203703612299307E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <f>B4-B5</f>
+        <v>0.14000000000942237</v>
+      </c>
+      <c r="C8" s="1">
+        <f>C4-C5</f>
+        <v>4.6574073981901165E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9.2499999816936906E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9.2499999816936906E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>